<commit_message>
commited some framework changes
THIS REVISION HAS THE LATEST WORKING MCU CODE
</commit_message>
<xml_diff>
--- a/Code/Hardware/instruction list.xlsx
+++ b/Code/Hardware/instruction list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="21015" windowHeight="9465"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="21015" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>description</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>if(a!=0)goto b;</t>
+  </si>
+  <si>
+    <t>c=a&lt;b;</t>
+  </si>
+  <si>
+    <t>c=a&gt;b;</t>
+  </si>
+  <si>
+    <t>smaller than</t>
+  </si>
+  <si>
+    <t>larget than</t>
   </si>
 </sst>
 </file>
@@ -479,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,6 +751,28 @@
       </c>
       <c r="C22" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>